<commit_message>
Back-end Authenticed Login + app
</commit_message>
<xml_diff>
--- a/Phân tích nghiệp vụ.xlsx
+++ b/Phân tích nghiệp vụ.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>Tác nhân</t>
   </si>
@@ -283,13 +283,40 @@
   </si>
   <si>
     <t>Multi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config all app _ tutorials </t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy template (Common) + CSS + JS -&gt; static </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routing View + App Root </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API - View process </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viết Login </t>
+  </si>
+  <si>
+    <t>Setup login required mixed</t>
+  </si>
+  <si>
+    <t>Copy base dir (template html outside)</t>
+  </si>
+  <si>
+    <t>Lesson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +332,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,8 +382,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -840,218 +879,221 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1068,6 +1110,98 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1092" name="Check Box 68" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1092"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Done</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1366,11 +1500,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,150 +1518,150 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="55"/>
+      <c r="C8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="56"/>
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="23" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1548,15 +1683,46 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1092" r:id="rId4" name="Check Box 68">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>685800</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,204 +1740,204 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="32"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="67"/>
+      <c r="E3" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36" t="s">
+      <c r="F3" s="67"/>
+      <c r="G3" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36" t="s">
+      <c r="H3" s="67"/>
+      <c r="I3" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="J3" s="62"/>
+    </row>
+    <row r="4" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
-    </row>
-    <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="41" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41" t="s">
+      <c r="H10" s="22"/>
+      <c r="I10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="42"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="53" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="53" t="s">
+      <c r="F11" s="36"/>
+      <c r="G11" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="53" t="s">
+      <c r="H11" s="36"/>
+      <c r="I11" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="55"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="42"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="47" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1787,10 +1953,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L24"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,302 +1967,308 @@
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="10.125" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="15" max="15" width="5.625" customWidth="1"/>
+    <col min="16" max="16" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="58"/>
-      <c r="C2" s="59" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="59" t="s">
+      <c r="J2" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="67" t="s">
+      <c r="L2" s="68" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="59" t="s">
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="61" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="61" t="s">
+      <c r="E3" s="44"/>
+      <c r="F3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="59" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="64" t="s">
+      <c r="H4" s="42"/>
+      <c r="I4" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="64" t="s">
+      <c r="J4" s="46" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="59" t="s">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="64" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="64" t="s">
+      <c r="I5" s="42"/>
+      <c r="J5" s="46" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="59" t="s">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="59" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="65" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="66" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="68" t="s">
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="71" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="70" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="70" t="s">
         <v>43</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="70" t="s">
         <v>44</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="71"/>
       <c r="C13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="70"/>
       <c r="L13" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="71"/>
       <c r="C14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="70"/>
       <c r="F14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="70"/>
       <c r="I14" s="2"/>
-      <c r="K14" s="3"/>
+      <c r="K14" s="70"/>
       <c r="L14" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="71"/>
       <c r="C15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="70"/>
       <c r="I15" s="2"/>
-      <c r="K15" s="3"/>
+      <c r="K15" s="70"/>
       <c r="L15" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="71"/>
       <c r="C16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="70"/>
       <c r="I16" s="2"/>
-      <c r="K16" s="3"/>
+      <c r="K16" s="70"/>
       <c r="L16" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="2"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="70"/>
       <c r="L17" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="2"/>
-      <c r="K18" s="3"/>
+      <c r="K18" s="70"/>
       <c r="L18" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="70" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="69" t="s">
         <v>76</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="69" t="s">
         <v>47</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="69" t="s">
         <v>48</v>
       </c>
       <c r="L20" s="2" t="s">
@@ -2103,69 +2276,85 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
+      <c r="B21" s="70"/>
       <c r="C21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="69"/>
       <c r="I21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K21" s="3"/>
+      <c r="K21" s="69"/>
       <c r="L21" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="69"/>
       <c r="I22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="69"/>
       <c r="L22" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
+      <c r="B23" s="70"/>
       <c r="C23" s="2"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="2"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="69"/>
       <c r="L23" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="2"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="2"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="69"/>
       <c r="I24" s="2"/>
-      <c r="K24" s="3"/>
+      <c r="K24" s="69"/>
       <c r="L24" s="2" t="s">
         <v>86</v>
       </c>
     </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="72"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="72"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="72"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="L2:P2"/>
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="E20:E24"/>
     <mergeCell ref="H20:H24"/>
@@ -2181,12 +2370,59 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="36.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>